<commit_message>
extract program from template
</commit_message>
<xml_diff>
--- a/pcor_tools/pcor_ingest/spreadsheet/pcor_geospatial_data_resource.xlsx
+++ b/pcor_tools/pcor_ingest/spreadsheet/pcor_geospatial_data_resource.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/conwaymc/Documents/workspace-pcor/pcor_gen3_artifacts/pcor_tools/pcor_ingest/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2533066-7F22-FD41-9010-0947773F2771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9860E38-8AB9-A74D-896B-FE2536D41500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12380" windowHeight="22400" xr2:uid="{0E637B2F-D201-6448-B8F7-9EEB771C5771}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35940" windowHeight="22400" xr2:uid="{0E637B2F-D201-6448-B8F7-9EEB771C5771}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -988,10 +988,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1294,7 +1290,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>